<commit_message>
Updated, functioning project example
</commit_message>
<xml_diff>
--- a/inst/extdata/sample_data_bread.xlsx
+++ b/inst/extdata/sample_data_bread.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\amp\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{265C4855-3387-4C59-9617-2BDF8EC66CDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B68DB7C-5DB1-46EB-8201-160EA2B204A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="2784" windowWidth="20244" windowHeight="16464" xr2:uid="{91434C08-245B-419E-81FD-4898C2CE7306}"/>
+    <workbookView xWindow="1164" yWindow="4272" windowWidth="20244" windowHeight="15984" xr2:uid="{91434C08-245B-419E-81FD-4898C2CE7306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -903,13 +903,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A26B25A-0DBA-42E5-A42D-467E2236D8AA}">
   <dimension ref="A1:HQ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" topLeftCell="GX1" workbookViewId="0">
+      <selection activeCell="HI20" sqref="HI20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:225" x14ac:dyDescent="0.3">
       <c r="X1" t="s">
         <v>1</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:225" x14ac:dyDescent="0.3">
       <c r="X2" t="s">
         <v>7</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:225" x14ac:dyDescent="0.3">
       <c r="X3" t="s">
         <v>0</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:225" x14ac:dyDescent="0.3">
       <c r="X4" t="s">
         <v>9</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>8673</v>
       </c>
       <c r="GH5">
-        <v>25865</v>
+        <v>0</v>
       </c>
       <c r="GI5">
         <v>13894</v>
@@ -4018,7 +4018,7 @@
         <v>66439</v>
       </c>
     </row>
-    <row r="6" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>50865</v>
       </c>
       <c r="FT6">
-        <v>76860</v>
+        <v>0</v>
       </c>
       <c r="FU6">
         <v>32193</v>
@@ -4551,7 +4551,7 @@
         <v>66209</v>
       </c>
       <c r="FX6">
-        <v>117230</v>
+        <v>0</v>
       </c>
       <c r="FY6">
         <v>44432</v>
@@ -4623,7 +4623,7 @@
         <v>10245</v>
       </c>
       <c r="GV6">
-        <v>12350</v>
+        <v>0</v>
       </c>
       <c r="GW6">
         <v>62828</v>
@@ -4653,7 +4653,7 @@
         <v>9965</v>
       </c>
       <c r="HF6">
-        <v>65169</v>
+        <v>0</v>
       </c>
       <c r="HG6">
         <v>35749</v>
@@ -4689,7 +4689,7 @@
         <v>87263</v>
       </c>
     </row>
-    <row r="7" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>239550</v>
       </c>
       <c r="BM7">
-        <v>280487</v>
+        <v>0</v>
       </c>
       <c r="BN7">
         <v>173969</v>
@@ -4886,7 +4886,7 @@
         <v>237393</v>
       </c>
       <c r="BP7">
-        <v>151266</v>
+        <v>0</v>
       </c>
       <c r="BQ7">
         <v>157804</v>
@@ -4904,7 +4904,7 @@
         <v>111390</v>
       </c>
       <c r="BV7">
-        <v>225336</v>
+        <v>0</v>
       </c>
       <c r="BW7">
         <v>179186</v>
@@ -5063,7 +5063,7 @@
         <v>187878</v>
       </c>
       <c r="DW7">
-        <v>189259</v>
+        <v>0</v>
       </c>
       <c r="DX7">
         <v>130887</v>
@@ -5087,7 +5087,7 @@
         <v>177119</v>
       </c>
       <c r="EE7">
-        <v>207377</v>
+        <v>0</v>
       </c>
       <c r="EF7">
         <v>175092</v>
@@ -5228,10 +5228,10 @@
         <v>178484</v>
       </c>
       <c r="FZ7">
-        <v>154457</v>
+        <v>0</v>
       </c>
       <c r="GA7">
-        <v>124873</v>
+        <v>0</v>
       </c>
       <c r="GB7">
         <v>177957</v>
@@ -5240,7 +5240,7 @@
         <v>124414</v>
       </c>
       <c r="GD7">
-        <v>143168</v>
+        <v>0</v>
       </c>
       <c r="GE7">
         <v>203939</v>
@@ -5255,7 +5255,7 @@
         <v>155753</v>
       </c>
       <c r="GI7">
-        <v>177015</v>
+        <v>0</v>
       </c>
       <c r="GJ7">
         <v>175649</v>
@@ -5312,7 +5312,7 @@
         <v>109495</v>
       </c>
       <c r="HB7">
-        <v>137123</v>
+        <v>0</v>
       </c>
       <c r="HC7">
         <v>170719</v>
@@ -5360,7 +5360,7 @@
         <v>147053</v>
       </c>
     </row>
-    <row r="8" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>242028</v>
       </c>
       <c r="AD8">
-        <v>202516</v>
+        <v>0</v>
       </c>
       <c r="AE8">
         <v>170631</v>
@@ -5578,7 +5578,7 @@
         <v>208327</v>
       </c>
       <c r="BW8">
-        <v>228785</v>
+        <v>0</v>
       </c>
       <c r="BX8">
         <v>89974</v>
@@ -5716,7 +5716,7 @@
         <v>240170</v>
       </c>
       <c r="DQ8">
-        <v>197388</v>
+        <v>0</v>
       </c>
       <c r="DR8">
         <v>276763</v>
@@ -5728,7 +5728,7 @@
         <v>272447</v>
       </c>
       <c r="DU8">
-        <v>173302</v>
+        <v>0</v>
       </c>
       <c r="DV8">
         <v>240328</v>
@@ -5881,10 +5881,10 @@
         <v>258271</v>
       </c>
       <c r="FT8">
-        <v>186363</v>
+        <v>0</v>
       </c>
       <c r="FU8">
-        <v>264553</v>
+        <v>0</v>
       </c>
       <c r="FV8">
         <v>231166</v>
@@ -5908,13 +5908,13 @@
         <v>232062</v>
       </c>
       <c r="GC8">
-        <v>182237</v>
+        <v>0</v>
       </c>
       <c r="GD8">
         <v>156620</v>
       </c>
       <c r="GE8">
-        <v>175592</v>
+        <v>0</v>
       </c>
       <c r="GF8">
         <v>218518</v>
@@ -5956,7 +5956,7 @@
         <v>190959</v>
       </c>
       <c r="GS8">
-        <v>39444</v>
+        <v>0</v>
       </c>
       <c r="GT8">
         <v>217982</v>
@@ -5980,7 +5980,7 @@
         <v>190449</v>
       </c>
       <c r="HA8">
-        <v>99757</v>
+        <v>0</v>
       </c>
       <c r="HB8">
         <v>214402</v>
@@ -6007,7 +6007,7 @@
         <v>171385</v>
       </c>
       <c r="HJ8">
-        <v>252385</v>
+        <v>0</v>
       </c>
       <c r="HK8">
         <v>164351</v>
@@ -6031,7 +6031,7 @@
         <v>208939</v>
       </c>
     </row>
-    <row r="9" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>499027</v>
       </c>
       <c r="AL9">
-        <v>509859</v>
+        <v>0</v>
       </c>
       <c r="AM9">
         <v>510937</v>
@@ -6231,7 +6231,7 @@
         <v>558841</v>
       </c>
       <c r="BQ9">
-        <v>543471</v>
+        <v>0</v>
       </c>
       <c r="BR9">
         <v>564282</v>
@@ -6411,7 +6411,7 @@
         <v>498480</v>
       </c>
       <c r="DY9">
-        <v>516885</v>
+        <v>0</v>
       </c>
       <c r="DZ9">
         <v>547038</v>
@@ -6426,10 +6426,10 @@
         <v>568860</v>
       </c>
       <c r="ED9">
-        <v>625997</v>
+        <v>0</v>
       </c>
       <c r="EE9">
-        <v>550620</v>
+        <v>0</v>
       </c>
       <c r="EF9">
         <v>569887</v>
@@ -6567,7 +6567,7 @@
         <v>499596</v>
       </c>
       <c r="FY9">
-        <v>531393</v>
+        <v>0</v>
       </c>
       <c r="FZ9">
         <v>533046</v>
@@ -6585,7 +6585,7 @@
         <v>535458</v>
       </c>
       <c r="GE9">
-        <v>497072</v>
+        <v>0</v>
       </c>
       <c r="GF9">
         <v>652269</v>
@@ -6702,7 +6702,7 @@
         <v>541110</v>
       </c>
     </row>
-    <row r="10" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>858355</v>
       </c>
       <c r="FY10">
-        <v>1645266</v>
+        <v>0</v>
       </c>
       <c r="FZ10">
         <v>1149408</v>
@@ -7301,7 +7301,7 @@
         <v>1163890</v>
       </c>
       <c r="GU10">
-        <v>687360</v>
+        <v>0</v>
       </c>
       <c r="GV10">
         <v>1410345</v>
@@ -7313,7 +7313,7 @@
         <v>169193</v>
       </c>
       <c r="GY10">
-        <v>914102</v>
+        <v>0</v>
       </c>
       <c r="GZ10">
         <v>332121</v>
@@ -7361,7 +7361,7 @@
         <v>382811</v>
       </c>
       <c r="HO10">
-        <v>1018896</v>
+        <v>0</v>
       </c>
       <c r="HP10">
         <v>331756</v>
@@ -7370,7 +7370,7 @@
         <v>1299401</v>
       </c>
     </row>
-    <row r="11" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>1549550</v>
       </c>
       <c r="AB11">
-        <v>1531848</v>
+        <v>0</v>
       </c>
       <c r="AC11">
         <v>1492557</v>
@@ -7987,7 +7987,7 @@
         <v>1364856</v>
       </c>
       <c r="GZ11">
-        <v>1511486</v>
+        <v>0</v>
       </c>
       <c r="HA11">
         <v>1281941</v>
@@ -8002,7 +8002,7 @@
         <v>1381223</v>
       </c>
       <c r="HE11">
-        <v>1241432</v>
+        <v>0</v>
       </c>
       <c r="HF11">
         <v>1425930</v>
@@ -8041,7 +8041,7 @@
         <v>1411237</v>
       </c>
     </row>
-    <row r="12" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>4084</v>
       </c>
       <c r="CA12">
-        <v>4780</v>
+        <v>0</v>
       </c>
       <c r="CB12">
         <v>6049</v>
@@ -8406,7 +8406,7 @@
         <v>4276</v>
       </c>
       <c r="DT12">
-        <v>12242</v>
+        <v>0</v>
       </c>
       <c r="DU12">
         <v>8874</v>
@@ -8568,7 +8568,7 @@
         <v>4180</v>
       </c>
       <c r="FV12">
-        <v>17470</v>
+        <v>0</v>
       </c>
       <c r="FW12">
         <v>3359</v>
@@ -8640,7 +8640,7 @@
         <v>13268</v>
       </c>
       <c r="GT12">
-        <v>17801</v>
+        <v>0</v>
       </c>
       <c r="GU12">
         <v>6371</v>
@@ -8712,7 +8712,7 @@
         <v>18745</v>
       </c>
     </row>
-    <row r="13" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>16174</v>
       </c>
     </row>
-    <row r="14" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>40059</v>
       </c>
       <c r="BS14">
-        <v>35693</v>
+        <v>0</v>
       </c>
       <c r="BT14">
         <v>36083</v>
@@ -9733,7 +9733,7 @@
         <v>24641</v>
       </c>
       <c r="DR14">
-        <v>8796</v>
+        <v>0</v>
       </c>
       <c r="DS14">
         <v>26646</v>
@@ -10045,7 +10045,7 @@
         <v>4436</v>
       </c>
     </row>
-    <row r="15" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>2686</v>
       </c>
     </row>
-    <row r="16" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>10022</v>
       </c>
     </row>
-    <row r="17" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>12062</v>
       </c>
       <c r="DV17">
-        <v>19605</v>
+        <v>0</v>
       </c>
       <c r="DW17">
         <v>27963</v>
@@ -11782,7 +11782,7 @@
         <v>15897</v>
       </c>
       <c r="ED17">
-        <v>21610</v>
+        <v>0</v>
       </c>
       <c r="EE17">
         <v>17258</v>
@@ -12058,7 +12058,7 @@
         <v>11246</v>
       </c>
     </row>
-    <row r="18" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -12660,7 +12660,7 @@
         <v>15991</v>
       </c>
       <c r="GU18">
-        <v>30159</v>
+        <v>0</v>
       </c>
       <c r="GV18">
         <v>14143</v>
@@ -12672,7 +12672,7 @@
         <v>19503</v>
       </c>
       <c r="GY18">
-        <v>8860</v>
+        <v>0</v>
       </c>
       <c r="GZ18">
         <v>15107</v>
@@ -12729,7 +12729,7 @@
         <v>15837</v>
       </c>
     </row>
-    <row r="19" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -13361,7 +13361,7 @@
         <v>8138</v>
       </c>
       <c r="HE19">
-        <v>9529</v>
+        <v>0</v>
       </c>
       <c r="HF19">
         <v>22588</v>
@@ -13400,7 +13400,7 @@
         <v>30021</v>
       </c>
     </row>
-    <row r="20" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>6149</v>
       </c>
       <c r="BW20">
-        <v>7682</v>
+        <v>0</v>
       </c>
       <c r="BX20">
         <v>11559</v>
@@ -14068,7 +14068,7 @@
         <v>17658</v>
       </c>
     </row>
-    <row r="21" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -14145,7 +14145,7 @@
         <v>31745</v>
       </c>
       <c r="AC21">
-        <v>23257</v>
+        <v>0</v>
       </c>
       <c r="AD21">
         <v>59419</v>
@@ -14166,7 +14166,7 @@
         <v>53310</v>
       </c>
       <c r="AJ21">
-        <v>29984</v>
+        <v>0</v>
       </c>
       <c r="AK21">
         <v>43984</v>
@@ -14430,7 +14430,7 @@
         <v>17107</v>
       </c>
       <c r="DT21">
-        <v>33645</v>
+        <v>0</v>
       </c>
       <c r="DU21">
         <v>62447</v>
@@ -14736,7 +14736,7 @@
         <v>40428</v>
       </c>
     </row>
-    <row r="22" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -15407,7 +15407,7 @@
         <v>95163</v>
       </c>
     </row>
-    <row r="23" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -15928,7 +15928,7 @@
         <v>45457</v>
       </c>
       <c r="FT23">
-        <v>68627</v>
+        <v>0</v>
       </c>
       <c r="FU23">
         <v>46557</v>
@@ -16003,7 +16003,7 @@
         <v>107165</v>
       </c>
       <c r="GS23">
-        <v>160730</v>
+        <v>0</v>
       </c>
       <c r="GT23">
         <v>43379</v>
@@ -16027,7 +16027,7 @@
         <v>67329</v>
       </c>
       <c r="HA23">
-        <v>82949</v>
+        <v>0</v>
       </c>
       <c r="HB23">
         <v>51836</v>
@@ -16078,7 +16078,7 @@
         <v>52396</v>
       </c>
     </row>
-    <row r="24" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -16449,7 +16449,7 @@
         <v>113339</v>
       </c>
       <c r="DW24">
-        <v>120756</v>
+        <v>0</v>
       </c>
       <c r="DX24">
         <v>124573</v>
@@ -16464,7 +16464,7 @@
         <v>98498</v>
       </c>
       <c r="EB24">
-        <v>27043</v>
+        <v>0</v>
       </c>
       <c r="EC24">
         <v>234084</v>
@@ -16746,7 +16746,7 @@
         <v>176849</v>
       </c>
     </row>
-    <row r="25" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -16838,7 +16838,7 @@
         <v>262404</v>
       </c>
       <c r="AG25">
-        <v>286447</v>
+        <v>0</v>
       </c>
       <c r="AH25">
         <v>229511</v>
@@ -16850,7 +16850,7 @@
         <v>99626</v>
       </c>
       <c r="AK25">
-        <v>168059</v>
+        <v>0</v>
       </c>
       <c r="AL25">
         <v>249573</v>
@@ -17126,7 +17126,7 @@
         <v>293681</v>
       </c>
       <c r="DY25">
-        <v>214440</v>
+        <v>0</v>
       </c>
       <c r="DZ25">
         <v>181186</v>
@@ -17417,7 +17417,7 @@
         <v>245000</v>
       </c>
     </row>
-    <row r="26" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -17611,7 +17611,7 @@
         <v>222512</v>
       </c>
       <c r="BO26">
-        <v>545123</v>
+        <v>0</v>
       </c>
       <c r="BP26">
         <v>111509</v>
@@ -18088,7 +18088,7 @@
         <v>530303</v>
       </c>
     </row>
-    <row r="27" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -18171,7 +18171,7 @@
         <v>270726</v>
       </c>
       <c r="AE27">
-        <v>252281</v>
+        <v>0</v>
       </c>
       <c r="AF27">
         <v>150907</v>
@@ -18756,7 +18756,7 @@
         <v>317985</v>
       </c>
     </row>
-    <row r="28" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -18983,7 +18983,7 @@
         <v>77397</v>
       </c>
       <c r="BZ28">
-        <v>102365</v>
+        <v>0</v>
       </c>
       <c r="CA28">
         <v>121838</v>
@@ -19109,7 +19109,7 @@
         <v>125603</v>
       </c>
       <c r="DP28">
-        <v>91038</v>
+        <v>0</v>
       </c>
       <c r="DQ28">
         <v>97893</v>
@@ -19427,7 +19427,7 @@
         <v>132687</v>
       </c>
     </row>
-    <row r="29" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -19498,7 +19498,7 @@
         <v>188518</v>
       </c>
       <c r="AA29">
-        <v>152622</v>
+        <v>0</v>
       </c>
       <c r="AB29">
         <v>90038</v>
@@ -20095,7 +20095,7 @@
         <v>109770</v>
       </c>
     </row>
-    <row r="30" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -20187,7 +20187,7 @@
         <v>247282</v>
       </c>
       <c r="AH30">
-        <v>187928</v>
+        <v>0</v>
       </c>
       <c r="AI30">
         <v>254670</v>
@@ -20202,7 +20202,7 @@
         <v>214782</v>
       </c>
       <c r="AM30">
-        <v>158398</v>
+        <v>0</v>
       </c>
       <c r="AN30">
         <v>149364</v>
@@ -20763,7 +20763,7 @@
         <v>164348</v>
       </c>
     </row>
-    <row r="31" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -21134,7 +21134,7 @@
         <v>148106</v>
       </c>
       <c r="DW31">
-        <v>135202</v>
+        <v>0</v>
       </c>
       <c r="DX31">
         <v>75768</v>
@@ -21431,7 +21431,7 @@
         <v>151819</v>
       </c>
     </row>
-    <row r="32" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -22102,7 +22102,7 @@
         <v>140016</v>
       </c>
     </row>
-    <row r="33" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -22770,7 +22770,7 @@
         <v>530303</v>
       </c>
     </row>
-    <row r="34" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -22979,7 +22979,7 @@
         <v>1565293</v>
       </c>
       <c r="BU34">
-        <v>1405760</v>
+        <v>0</v>
       </c>
       <c r="BV34">
         <v>2068090</v>
@@ -23438,7 +23438,7 @@
         <v>1558239</v>
       </c>
     </row>
-    <row r="35" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -24106,7 +24106,7 @@
         <v>156682</v>
       </c>
     </row>
-    <row r="36" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -24774,7 +24774,7 @@
         <v>372222</v>
       </c>
     </row>
-    <row r="37" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -24863,7 +24863,7 @@
         <v>122050</v>
       </c>
       <c r="AG37">
-        <v>236805</v>
+        <v>0</v>
       </c>
       <c r="AH37">
         <v>106591</v>
@@ -25442,7 +25442,7 @@
         <v>347823</v>
       </c>
     </row>
-    <row r="38" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -26110,7 +26110,7 @@
         <v>129776</v>
       </c>
     </row>
-    <row r="39" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -26778,7 +26778,7 @@
         <v>317350</v>
       </c>
     </row>
-    <row r="40" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -27449,7 +27449,7 @@
         <v>193083</v>
       </c>
     </row>
-    <row r="41" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -28117,7 +28117,7 @@
         <v>134493</v>
       </c>
     </row>
-    <row r="42" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -28788,7 +28788,7 @@
         <v>231586</v>
       </c>
     </row>
-    <row r="43" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -29456,7 +29456,7 @@
         <v>238221</v>
       </c>
     </row>
-    <row r="44" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -30124,7 +30124,7 @@
         <v>175664</v>
       </c>
     </row>
-    <row r="45" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -30792,7 +30792,7 @@
         <v>149113</v>
       </c>
     </row>
-    <row r="46" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -31460,7 +31460,7 @@
         <v>208656</v>
       </c>
     </row>
-    <row r="47" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -32131,7 +32131,7 @@
         <v>23112</v>
       </c>
     </row>
-    <row r="48" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -32799,7 +32799,7 @@
         <v>52368</v>
       </c>
     </row>
-    <row r="49" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -33467,7 +33467,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="50" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -34135,7 +34135,7 @@
         <v>9134</v>
       </c>
     </row>
-    <row r="51" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -34803,7 +34803,7 @@
         <v>17071</v>
       </c>
     </row>
-    <row r="52" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -35471,7 +35471,7 @@
         <v>6013</v>
       </c>
     </row>
-    <row r="53" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -36136,7 +36136,7 @@
         <v>59180</v>
       </c>
     </row>
-    <row r="54" spans="1:225" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:225" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>34</v>
       </c>

</xml_diff>